<commit_message>
Long Form Latest Code
Test
</commit_message>
<xml_diff>
--- a/LongForm_TeamB/ExcelFile/API_inputs.xlsx
+++ b/LongForm_TeamB/ExcelFile/API_inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14775" windowHeight="3585" tabRatio="903" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14265" windowHeight="1680" tabRatio="903" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="RLtoWOPMappingRule" sheetId="12" state="hidden" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <sheet name="MP" sheetId="15" state="hidden" r:id="rId25"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A2:G11"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -1341,7 +1341,7 @@
 AND Source_System='AMCN.EVERTZ.MEDIATOR.REGISTRATION.TO.ADAPTER'</t>
   </si>
   <si>
-    <t>RLA177301</t>
+    <t>RLA177308</t>
   </si>
 </sst>
 </file>
@@ -2177,7 +2177,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Revert "Latest SF Code"
This reverts commit 3fdc0baa3352e7d26f963ae282cd7aa3898eac4e.
</commit_message>
<xml_diff>
--- a/LongForm_TeamB/ExcelFile/API_inputs.xlsx
+++ b/LongForm_TeamB/ExcelFile/API_inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14730" windowHeight="6060" tabRatio="903" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15435" windowHeight="2415" tabRatio="903" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="RLtoWOPMappingRule" sheetId="12" state="hidden" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="MP" sheetId="15" state="hidden" r:id="rId24"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G17"/>
+  <oleSize ref="A1:G14"/>
 </workbook>
 </file>
 
@@ -1303,6 +1303,9 @@
     <t>adamqa</t>
   </si>
   <si>
+    <t>amcnTest@123</t>
+  </si>
+  <si>
     <t>DataBaseURL</t>
   </si>
   <si>
@@ -1328,13 +1331,10 @@
     <t>3</t>
   </si>
   <si>
-    <t>amcnTest@456</t>
-  </si>
-  <si>
-    <t>Amc@2020</t>
-  </si>
-  <si>
-    <t>RLA172954</t>
+    <t>Symbox@457</t>
+  </si>
+  <si>
+    <t>RLA178227</t>
   </si>
 </sst>
 </file>
@@ -2216,7 +2216,7 @@
         <v>367</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -2604,7 +2604,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="409.6">
       <c r="D6" s="3"/>
     </row>
   </sheetData>
@@ -4481,7 +4481,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4550,7 +4550,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4563,7 +4563,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="41" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>144</v>
@@ -4572,7 +4572,7 @@
         <v>99</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="6" customFormat="1" ht="189">
@@ -4582,19 +4582,16 @@
       <c r="B2" s="47" t="s">
         <v>389</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>395</v>
+      <c r="C2" s="47" t="s">
+        <v>390</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4711,7 +4708,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4777,7 +4774,7 @@
         <v>374</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="F2" s="43" t="s">
         <v>382</v>

</xml_diff>